<commit_message>
Modified Demos from ECP3004
</commit_message>
<xml_diff>
--- a/demo_12_PP_Ch_10_Read_Write/empty_files/empty_worksheet.xlsx
+++ b/demo_12_PP_Ch_10_Read_Write/empty_files/empty_worksheet.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>A</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,18 +333,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>